<commit_message>
monthly budget file for 13, 14, 15, 16, 17 lessons
</commit_message>
<xml_diff>
--- a/First.xlsx
+++ b/First.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\moin\Excel Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8322745C-A750-40EE-A7B4-16721CB63F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADF1F93-A398-4705-B910-0856998C1948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE21FD99-2659-4CF8-BD58-F111F1F6C8BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Completed Lessons" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Shortcut Keys" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Episode 1</t>
   </si>
@@ -136,6 +136,21 @@
   </si>
   <si>
     <t>Common Excel Shortcut Keys</t>
+  </si>
+  <si>
+    <t>Entering Text to Create Spreadsheet Titles</t>
+  </si>
+  <si>
+    <t>Working with Numeric Data in Excel</t>
+  </si>
+  <si>
+    <t>Entering Date Values in Excel</t>
+  </si>
+  <si>
+    <t>Working with Cell References</t>
+  </si>
+  <si>
+    <t>Creating Basic Formulas in Excel</t>
   </si>
 </sst>
 </file>
@@ -510,7 +525,7 @@
   <dimension ref="B1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -629,33 +644,48 @@
       <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="C14" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="15" spans="2:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="C15" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" spans="2:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
monthly budget file for 13, 14, 15, 16, 17 and 18 lessons
</commit_message>
<xml_diff>
--- a/First.xlsx
+++ b/First.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\moin\Excel Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8322745C-A750-40EE-A7B4-16721CB63F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADF1F93-A398-4705-B910-0856998C1948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE21FD99-2659-4CF8-BD58-F111F1F6C8BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Completed Lessons" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Shortcut Keys" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Episode 1</t>
   </si>
@@ -136,6 +136,21 @@
   </si>
   <si>
     <t>Common Excel Shortcut Keys</t>
+  </si>
+  <si>
+    <t>Entering Text to Create Spreadsheet Titles</t>
+  </si>
+  <si>
+    <t>Working with Numeric Data in Excel</t>
+  </si>
+  <si>
+    <t>Entering Date Values in Excel</t>
+  </si>
+  <si>
+    <t>Working with Cell References</t>
+  </si>
+  <si>
+    <t>Creating Basic Formulas in Excel</t>
   </si>
 </sst>
 </file>
@@ -510,7 +525,7 @@
   <dimension ref="B1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -629,33 +644,48 @@
       <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="C14" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="15" spans="2:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="C15" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" spans="2:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>30</v>
       </c>

</xml_diff>